<commit_message>
veritly ai demo project with Visuals
</commit_message>
<xml_diff>
--- a/data/derived/churn_analysis_v1.xlsx
+++ b/data/derived/churn_analysis_v1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>With Voicemail Plan</t>
+          <t>With Voice Mail Plan</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -540,7 +540,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Without Voicemail Plan</t>
+          <t>Without Voice Mail Plan</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -556,226 +556,186 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Intl Minutes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>Threshold: 3.9</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>26.47</v>
-      </c>
-      <c r="D7" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" t="n">
-        <v>34</v>
-      </c>
+        <v>14.68</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Intl Charge</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>Threshold: 1.05</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>26.47</v>
-      </c>
-      <c r="D8" t="n">
-        <v>18</v>
-      </c>
-      <c r="E8" t="n">
-        <v>68</v>
-      </c>
+        <v>14.68</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Day Minutes</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>Threshold: 291.2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D9" t="n">
-        <v>18</v>
-      </c>
-      <c r="E9" t="n">
-        <v>72</v>
-      </c>
+        <v>75.38</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Day Charge</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>Threshold: 49.5</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>24.29</v>
-      </c>
-      <c r="D10" t="n">
-        <v>17</v>
-      </c>
-      <c r="E10" t="n">
-        <v>70</v>
-      </c>
+        <v>75.38</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Customer Service Calls</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>Threshold: 5</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>23.33</v>
-      </c>
-      <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="n">
-        <v>60</v>
-      </c>
+        <v>61.39</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: International Plan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MI</t>
+          <t>Threshold: 1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21.92</v>
-      </c>
-      <c r="D12" t="n">
-        <v>16</v>
-      </c>
-      <c r="E12" t="n">
-        <v>73</v>
-      </c>
+        <v>42.41</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Night Minutes</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>Threshold: 104.9</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>21.54</v>
-      </c>
-      <c r="D13" t="n">
-        <v>14</v>
-      </c>
-      <c r="E13" t="n">
-        <v>65</v>
-      </c>
+        <v>14.77</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Night Charge</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>Threshold: 4.72</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>21.21</v>
-      </c>
-      <c r="D14" t="n">
-        <v>14</v>
-      </c>
-      <c r="E14" t="n">
-        <v>66</v>
-      </c>
+        <v>14.76</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Eve Minutes</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>Threshold: 301.0</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>21.21</v>
-      </c>
-      <c r="D15" t="n">
-        <v>14</v>
-      </c>
-      <c r="E15" t="n">
-        <v>66</v>
-      </c>
+        <v>29.76</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Churn Rate by top_states_by_churn</t>
+          <t>Tipping Point: Total Eve Charge</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ME</t>
+          <t>Threshold: 25.59</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>20.97</v>
-      </c>
-      <c r="D16" t="n">
-        <v>13</v>
-      </c>
-      <c r="E16" t="n">
-        <v>62</v>
-      </c>
+        <v>29.76</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tipping Point: Customer Service Calls</t>
+          <t>Tipping Point: Account Length</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Threshold: 4</t>
+          <t>Threshold: 17</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>51.69</v>
+        <v>14.58</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
@@ -783,19 +743,87 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tipping Point: High Day Usage</t>
+          <t>Tipping Point: Total Day Calls</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Threshold: 216.4</t>
+          <t>Threshold: 141</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>29.29</v>
+        <v>20</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Model Accuracy</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>sklearn.LogisticRegression</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>86.34999999999999</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Model Precision</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>sklearn.metrics</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>57.69</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Model Recall</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>sklearn.metrics</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>21.74</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>High Risk Count</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>prob &gt; 0.5</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>834</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>